<commit_message>
Change question properties to .xls
</commit_message>
<xml_diff>
--- a/spreadsheet/Question_properties.xlsx
+++ b/spreadsheet/Question_properties.xlsx
@@ -9769,45 +9769,6 @@
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
 <headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*" guid="{C9E3B4C8-A12F-504A-8F75-627A9D8DE348}" diskRevisions="1" revisionId="8329" version="3">
-  <header guid="{24944B09-EC98-3540-A369-A00B990EC668}" dateTime="2013-05-25T15:59:44" maxSheetId="10" userName="David Belavy" r:id="rId62" minRId="8311" maxRId="8320">
-    <sheetIdMap count="9">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-      <sheetId val="5"/>
-      <sheetId val="6"/>
-      <sheetId val="7"/>
-      <sheetId val="8"/>
-      <sheetId val="9"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{4747004E-8CF4-834F-9B05-CA802EFA6EF1}" dateTime="2013-05-25T16:00:16" maxSheetId="10" userName="David Belavy" r:id="rId63">
-    <sheetIdMap count="9">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-      <sheetId val="5"/>
-      <sheetId val="6"/>
-      <sheetId val="7"/>
-      <sheetId val="8"/>
-      <sheetId val="9"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{8611A6FC-4819-3240-8DA3-FC37F0049008}" dateTime="2013-05-25T16:13:21" maxSheetId="10" userName="David Belavy" r:id="rId64" minRId="8321" maxRId="8327">
-    <sheetIdMap count="9">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-      <sheetId val="5"/>
-      <sheetId val="6"/>
-      <sheetId val="7"/>
-      <sheetId val="8"/>
-      <sheetId val="9"/>
-    </sheetIdMap>
-  </header>
   <header guid="{2AA0907F-9791-DA40-A28F-1D6EEFF16D18}" dateTime="2013-06-23T13:04:33" maxSheetId="10" userName="David Belavy" r:id="rId65" minRId="8328">
     <sheetIdMap count="9">
       <sheetId val="1"/>
@@ -9873,266 +9834,6 @@
 
 <file path=xl/revisions/revisionLog11.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <rcv guid="{A2822BA0-8792-8A42-8107-58F529CC73B7}" action="delete"/>
-  <rcv guid="{A2822BA0-8792-8A42-8107-58F529CC73B7}" action="add"/>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog15.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <rrc rId="8311" sId="5" ref="A108:XFD108" action="insertRow"/>
-  <rm rId="8312" sheetId="5" source="A109:XFD109" destination="A108:XFD108" sourceSheetId="5">
-    <rfmt sheetId="5" xfDxf="1" s="1" sqref="A108:XFD108" start="0" length="0">
-      <dxf>
-        <font>
-          <b val="0"/>
-          <i val="0"/>
-          <strike val="0"/>
-          <condense val="0"/>
-          <extend val="0"/>
-          <outline val="0"/>
-          <shadow val="0"/>
-          <u val="none"/>
-          <vertAlign val="baseline"/>
-          <sz val="10"/>
-          <color auto="1"/>
-          <name val="Calibri"/>
-          <scheme val="none"/>
-        </font>
-        <numFmt numFmtId="0" formatCode="General"/>
-        <fill>
-          <patternFill patternType="none">
-            <fgColor indexed="64"/>
-            <bgColor indexed="65"/>
-          </patternFill>
-        </fill>
-        <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-        <border diagonalUp="0" diagonalDown="0" outline="0">
-          <left/>
-          <right/>
-          <top/>
-          <bottom/>
-        </border>
-        <protection locked="1" hidden="0"/>
-      </dxf>
-    </rfmt>
-    <rfmt sheetId="5" sqref="A108" start="0" length="0">
-      <dxf>
-        <font>
-          <color indexed="8"/>
-          <name val="Calibri"/>
-          <scheme val="none"/>
-        </font>
-        <alignment vertical="bottom" readingOrder="0"/>
-      </dxf>
-    </rfmt>
-    <rfmt sheetId="5" sqref="B108" start="0" length="0">
-      <dxf>
-        <font>
-          <color indexed="8"/>
-          <name val="Calibri"/>
-          <scheme val="none"/>
-        </font>
-        <alignment horizontal="center" vertical="bottom" readingOrder="0"/>
-      </dxf>
-    </rfmt>
-    <rfmt sheetId="5" sqref="C108" start="0" length="0">
-      <dxf>
-        <font>
-          <color indexed="8"/>
-          <name val="Calibri"/>
-          <scheme val="none"/>
-        </font>
-        <alignment vertical="bottom" readingOrder="0"/>
-      </dxf>
-    </rfmt>
-    <rfmt sheetId="5" sqref="D108" start="0" length="0">
-      <dxf>
-        <font>
-          <color indexed="8"/>
-          <name val="Calibri"/>
-          <scheme val="none"/>
-        </font>
-        <alignment vertical="bottom" readingOrder="0"/>
-      </dxf>
-    </rfmt>
-  </rm>
-  <rcc rId="8313" sId="5" odxf="1" dxf="1">
-    <nc r="A109" t="inlineStr">
-      <is>
-        <t>Dental_status_patient</t>
-        <phoneticPr fontId="31" type="noConversion"/>
-      </is>
-    </nc>
-    <odxf>
-      <font>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment vertical="center" readingOrder="0"/>
-    </odxf>
-    <ndxf>
-      <font>
-        <color indexed="8"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment vertical="bottom" readingOrder="0"/>
-    </ndxf>
-  </rcc>
-  <rfmt sheetId="5" sqref="B109" start="0" length="0">
-    <dxf>
-      <font>
-        <color indexed="8"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment vertical="bottom" readingOrder="0"/>
-    </dxf>
-  </rfmt>
-  <rcc rId="8314" sId="5">
-    <nc r="B109">
-      <v>8</v>
-    </nc>
-  </rcc>
-  <rcc rId="8315" sId="5">
-    <nc r="C109" t="inlineStr">
-      <is>
-        <t>None of the above</t>
-        <phoneticPr fontId="31" type="noConversion"/>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="8316" sId="5">
-    <nc r="D109" t="inlineStr">
-      <is>
-        <t>No prostheses or dental damage</t>
-        <phoneticPr fontId="31" type="noConversion"/>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="8317" sId="5">
-    <oc r="C102" t="inlineStr">
-      <is>
-        <t>Loose tooth or teeth</t>
-        <phoneticPr fontId="31" type="noConversion"/>
-      </is>
-    </oc>
-    <nc r="C102" t="inlineStr">
-      <is>
-        <t>Loose tooth (or teeth)</t>
-        <phoneticPr fontId="31" type="noConversion"/>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="8318" sId="5">
-    <oc r="C103" t="inlineStr">
-      <is>
-        <t>Chipped or broken tooth or teeth</t>
-        <phoneticPr fontId="31" type="noConversion"/>
-      </is>
-    </oc>
-    <nc r="C103" t="inlineStr">
-      <is>
-        <t>Chipped or broken tooth (or teeth)</t>
-        <phoneticPr fontId="31" type="noConversion"/>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="8319" sId="5">
-    <oc r="D103" t="inlineStr">
-      <is>
-        <t>Chipped or broken tooth or teeth</t>
-        <phoneticPr fontId="31" type="noConversion"/>
-      </is>
-    </oc>
-    <nc r="D103" t="inlineStr">
-      <is>
-        <t>Chipped or broken tooth (or teeth)</t>
-        <phoneticPr fontId="31" type="noConversion"/>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="8320" sId="5">
-    <oc r="D102" t="inlineStr">
-      <is>
-        <t>Loose tooth or teeth</t>
-        <phoneticPr fontId="31" type="noConversion"/>
-      </is>
-    </oc>
-    <nc r="D102" t="inlineStr">
-      <is>
-        <t>Loose tooth (or teeth)</t>
-        <phoneticPr fontId="31" type="noConversion"/>
-      </is>
-    </nc>
-  </rcc>
-  <rcv guid="{A2822BA0-8792-8A42-8107-58F529CC73B7}" action="delete"/>
-  <rcv guid="{A2822BA0-8792-8A42-8107-58F529CC73B7}" action="add"/>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog16.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <rcv guid="{A2822BA0-8792-8A42-8107-58F529CC73B7}" action="delete"/>
-  <rcv guid="{A2822BA0-8792-8A42-8107-58F529CC73B7}" action="add"/>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog17.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <rcc rId="8321" sId="5">
-    <oc r="C109" t="inlineStr">
-      <is>
-        <t>None of the above</t>
-        <phoneticPr fontId="31" type="noConversion"/>
-      </is>
-    </oc>
-    <nc r="C109" t="inlineStr">
-      <is>
-        <t>None of the above, no tooth problems or protheses.</t>
-        <phoneticPr fontId="31" type="noConversion"/>
-      </is>
-    </nc>
-  </rcc>
-  <rrc rId="8322" sId="5" ref="A109:XFD109" action="insertRow"/>
-  <rcc rId="8323" sId="5">
-    <nc r="A109" t="inlineStr">
-      <is>
-        <t>Dental_status_patient</t>
-        <phoneticPr fontId="31" type="noConversion"/>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="8324" sId="5">
-    <nc r="B109">
-      <v>8</v>
-    </nc>
-  </rcc>
-  <rcc rId="8325" sId="5">
-    <oc r="B110">
-      <v>8</v>
-    </oc>
-    <nc r="B110">
-      <v>9</v>
-    </nc>
-  </rcc>
-  <rcc rId="8326" sId="5">
-    <nc r="C109" t="inlineStr">
-      <is>
-        <t>Fillings</t>
-        <phoneticPr fontId="31" type="noConversion"/>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="8327" sId="5">
-    <nc r="D109" t="inlineStr">
-      <is>
-        <t>Fillings</t>
-        <phoneticPr fontId="31" type="noConversion"/>
-      </is>
-    </nc>
-  </rcc>
   <rcv guid="{A2822BA0-8792-8A42-8107-58F529CC73B7}" action="delete"/>
   <rcv guid="{A2822BA0-8792-8A42-8107-58F529CC73B7}" action="add"/>
 </revisions>

</xml_diff>